<commit_message>
MIDDLE OF DEV 17-2 jan
</commit_message>
<xml_diff>
--- a/MidiConverters/src/org/jjazz/midiconverters/resources/MidiStandardJJazzLab-DATA.xlsx
+++ b/MidiConverters/src/org/jjazz/midiconverters/resources/MidiStandardJJazzLab-DATA.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lelasseux\Documents\Perso\src\work\JJazzLab-X\MidiConverters\src\org\jjazz\midiconverters\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB4647F-DC4D-4832-9B7E-E2EB391FC5F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="1532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4436" uniqueCount="1590">
   <si>
     <t>Bank Number</t>
   </si>
@@ -4622,12 +4616,186 @@
   </si>
   <si>
     <t xml:space="preserve">        "Taisho kin"</t>
+  </si>
+  <si>
+    <t>Drum Kit Standard</t>
+  </si>
+  <si>
+    <t>Drum Kit Room</t>
+  </si>
+  <si>
+    <t>Drum Kit Power</t>
+  </si>
+  <si>
+    <t>Drum Kit Electronic</t>
+  </si>
+  <si>
+    <t>Drum Kit Analog</t>
+  </si>
+  <si>
+    <t>Drum Kit Jazz</t>
+  </si>
+  <si>
+    <t>Drum Kit Brush</t>
+  </si>
+  <si>
+    <t>Drum Kit Orchestra</t>
+  </si>
+  <si>
+    <t>Drum Kit SFX</t>
+  </si>
+  <si>
+    <t>Std1 Kit</t>
+  </si>
+  <si>
+    <t>Std2 Kit</t>
+  </si>
+  <si>
+    <t>Dry Kit</t>
+  </si>
+  <si>
+    <t>Bright Kit</t>
+  </si>
+  <si>
+    <t>Skim Kit</t>
+  </si>
+  <si>
+    <t>Slim Kit</t>
+  </si>
+  <si>
+    <t>Rogue Kit</t>
+  </si>
+  <si>
+    <t>Hob Kit</t>
+  </si>
+  <si>
+    <t>Room Kit</t>
+  </si>
+  <si>
+    <t>Dark Kit</t>
+  </si>
+  <si>
+    <t>Rock_Old Kit</t>
+  </si>
+  <si>
+    <t>Rock_Old2 Kit</t>
+  </si>
+  <si>
+    <t>Electro Kit</t>
+  </si>
+  <si>
+    <t>Analog Kit</t>
+  </si>
+  <si>
+    <t>Analog2 Kit</t>
+  </si>
+  <si>
+    <t>Dance Kit</t>
+  </si>
+  <si>
+    <t>Hiphop Kit</t>
+  </si>
+  <si>
+    <t>Jungle Kit</t>
+  </si>
+  <si>
+    <t>Apogee Kit</t>
+  </si>
+  <si>
+    <t>Perigee Kit</t>
+  </si>
+  <si>
+    <t>Jazz Kit</t>
+  </si>
+  <si>
+    <t>Jazz2 Kit</t>
+  </si>
+  <si>
+    <t>Brush Kit</t>
+  </si>
+  <si>
+    <t>Real_Brush Kit</t>
+  </si>
+  <si>
+    <t>Symphony Kit</t>
+  </si>
+  <si>
+    <t>HipHop2 Kit</t>
+  </si>
+  <si>
+    <t>Break Kit</t>
+  </si>
+  <si>
+    <t>Tramp Kit</t>
+  </si>
+  <si>
+    <t>Amber Kit</t>
+  </si>
+  <si>
+    <t>Coffin Kit</t>
+  </si>
+  <si>
+    <t>Live_Std Kit</t>
+  </si>
+  <si>
+    <t>Live_Funk Kit</t>
+  </si>
+  <si>
+    <t>Live_Brush Kit</t>
+  </si>
+  <si>
+    <t>Live_Std_Perc Kit</t>
+  </si>
+  <si>
+    <t>Live_Funk_Perc Kit</t>
+  </si>
+  <si>
+    <t>Live_Brush_Perc Kit</t>
+  </si>
+  <si>
+    <t>SFX1 Kit</t>
+  </si>
+  <si>
+    <t>SFX2 Kit</t>
+  </si>
+  <si>
+    <t>Techno_KS Kit</t>
+  </si>
+  <si>
+    <t>Techno_HI Kit</t>
+  </si>
+  <si>
+    <t>Techno_LO Kit</t>
+  </si>
+  <si>
+    <t>Sakura Kit</t>
+  </si>
+  <si>
+    <t>Small_Latin Kit</t>
+  </si>
+  <si>
+    <t>China Kit</t>
+  </si>
+  <si>
+    <t>Cuban Kit</t>
+  </si>
+  <si>
+    <t>Cuban2 Kit</t>
+  </si>
+  <si>
+    <t>Brazilian Kit</t>
+  </si>
+  <si>
+    <t>PopLatin1 Kit</t>
+  </si>
+  <si>
+    <t>PopLatin2 Kit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4645,7 +4813,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4655,6 +4823,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4686,7 +4866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4701,6 +4881,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4761,7 +4943,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4794,26 +4976,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4846,23 +5011,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5038,12 +5186,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F775"/>
   <sheetViews>
-    <sheetView topLeftCell="A689" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C773"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20552,7 +20700,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F775" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:F775">
     <filterColumn colId="5">
       <filters>
         <filter val="o"/>
@@ -20565,17 +20713,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I257"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I266"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I1048576"/>
+    <sheetView topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="E258" sqref="E258:F266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" customWidth="1"/>
   </cols>
@@ -27727,6 +27875,132 @@
         <v>3</v>
       </c>
     </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>222</v>
+      </c>
+      <c r="B258" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E258">
+        <v>256</v>
+      </c>
+      <c r="F258" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>223</v>
+      </c>
+      <c r="B259" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E259">
+        <v>257</v>
+      </c>
+      <c r="F259" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>224</v>
+      </c>
+      <c r="B260" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E260">
+        <v>258</v>
+      </c>
+      <c r="F260" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>225</v>
+      </c>
+      <c r="B261" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E261">
+        <v>259</v>
+      </c>
+      <c r="F261" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>226</v>
+      </c>
+      <c r="B262" t="s">
+        <v>1536</v>
+      </c>
+      <c r="E262">
+        <v>260</v>
+      </c>
+      <c r="F262" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>227</v>
+      </c>
+      <c r="B263" t="s">
+        <v>1537</v>
+      </c>
+      <c r="E263">
+        <v>261</v>
+      </c>
+      <c r="F263" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>228</v>
+      </c>
+      <c r="B264" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E264">
+        <v>262</v>
+      </c>
+      <c r="F264" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>229</v>
+      </c>
+      <c r="B265" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E265">
+        <v>263</v>
+      </c>
+      <c r="F265" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>230</v>
+      </c>
+      <c r="B266" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E266">
+        <v>264</v>
+      </c>
+      <c r="F266" t="s">
+        <v>1540</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -27734,11 +28008,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K481"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K530"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
+      <selection activeCell="H512" sqref="H512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40501,6 +40775,632 @@
         <v>115</v>
       </c>
     </row>
+    <row r="482" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A482" s="7">
+        <v>256</v>
+      </c>
+      <c r="B482" s="7" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G482">
+        <v>480</v>
+      </c>
+      <c r="H482" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A483" s="7">
+        <v>256</v>
+      </c>
+      <c r="B483" s="7"/>
+      <c r="G483">
+        <v>481</v>
+      </c>
+      <c r="H483" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A484" s="7">
+        <v>256</v>
+      </c>
+      <c r="B484" s="7"/>
+      <c r="G484">
+        <v>482</v>
+      </c>
+      <c r="H484" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="485" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A485" s="7">
+        <v>256</v>
+      </c>
+      <c r="B485" s="7"/>
+      <c r="G485">
+        <v>483</v>
+      </c>
+      <c r="H485" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="486" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A486" s="7">
+        <v>256</v>
+      </c>
+      <c r="B486" s="7"/>
+      <c r="G486">
+        <v>484</v>
+      </c>
+      <c r="H486" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="487" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A487" s="7">
+        <v>256</v>
+      </c>
+      <c r="B487" s="7"/>
+      <c r="G487">
+        <v>485</v>
+      </c>
+      <c r="H487" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A488" s="7">
+        <v>256</v>
+      </c>
+      <c r="B488" s="7"/>
+      <c r="G488">
+        <v>486</v>
+      </c>
+      <c r="H488" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A489" s="7">
+        <v>256</v>
+      </c>
+      <c r="B489" s="7"/>
+      <c r="G489">
+        <v>487</v>
+      </c>
+      <c r="H489" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="490" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A490" s="7">
+        <v>257</v>
+      </c>
+      <c r="B490" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G490">
+        <v>488</v>
+      </c>
+      <c r="H490" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="491" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A491" s="7">
+        <v>257</v>
+      </c>
+      <c r="B491" s="7"/>
+      <c r="G491">
+        <v>489</v>
+      </c>
+      <c r="H491" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A492" s="7">
+        <v>258</v>
+      </c>
+      <c r="B492" s="7" t="s">
+        <v>1534</v>
+      </c>
+      <c r="G492">
+        <v>490</v>
+      </c>
+      <c r="H492" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A493" s="7">
+        <v>258</v>
+      </c>
+      <c r="B493" s="7"/>
+      <c r="G493">
+        <v>491</v>
+      </c>
+      <c r="H493" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="494" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A494" s="7">
+        <v>259</v>
+      </c>
+      <c r="B494" s="7" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G494">
+        <v>492</v>
+      </c>
+      <c r="H494" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="495" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A495" s="7">
+        <v>260</v>
+      </c>
+      <c r="B495" s="7" t="s">
+        <v>1536</v>
+      </c>
+      <c r="G495">
+        <v>493</v>
+      </c>
+      <c r="H495" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A496" s="7">
+        <v>260</v>
+      </c>
+      <c r="B496" s="7"/>
+      <c r="G496">
+        <v>494</v>
+      </c>
+      <c r="H496" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A497" s="7">
+        <v>260</v>
+      </c>
+      <c r="B497" s="7"/>
+      <c r="G497">
+        <v>495</v>
+      </c>
+      <c r="H497" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A498" s="7">
+        <v>260</v>
+      </c>
+      <c r="B498" s="7"/>
+      <c r="G498">
+        <v>496</v>
+      </c>
+      <c r="H498" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A499" s="7">
+        <v>260</v>
+      </c>
+      <c r="B499" s="7"/>
+      <c r="G499">
+        <v>497</v>
+      </c>
+      <c r="H499" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A500" s="7">
+        <v>260</v>
+      </c>
+      <c r="B500" s="7"/>
+      <c r="G500">
+        <v>498</v>
+      </c>
+      <c r="H500" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A501" s="7">
+        <v>260</v>
+      </c>
+      <c r="B501" s="7"/>
+      <c r="G501">
+        <v>499</v>
+      </c>
+      <c r="H501" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A502" s="7">
+        <v>261</v>
+      </c>
+      <c r="B502" s="7" t="s">
+        <v>1537</v>
+      </c>
+      <c r="G502">
+        <v>500</v>
+      </c>
+      <c r="H502" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A503" s="7">
+        <v>261</v>
+      </c>
+      <c r="B503" s="7"/>
+      <c r="G503">
+        <v>501</v>
+      </c>
+      <c r="H503" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A504" s="7">
+        <v>262</v>
+      </c>
+      <c r="B504" s="7" t="s">
+        <v>1538</v>
+      </c>
+      <c r="G504">
+        <v>502</v>
+      </c>
+      <c r="H504" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A505" s="7">
+        <v>262</v>
+      </c>
+      <c r="B505" s="7"/>
+      <c r="G505">
+        <v>503</v>
+      </c>
+      <c r="H505" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A506" s="7">
+        <v>263</v>
+      </c>
+      <c r="B506" s="7" t="s">
+        <v>1539</v>
+      </c>
+      <c r="G506">
+        <v>504</v>
+      </c>
+      <c r="H506" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A507" s="7">
+        <v>259</v>
+      </c>
+      <c r="B507" s="7" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G507">
+        <v>505</v>
+      </c>
+      <c r="H507" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A508" s="7">
+        <v>259</v>
+      </c>
+      <c r="B508" s="7"/>
+      <c r="G508">
+        <v>506</v>
+      </c>
+      <c r="H508" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A509" s="7">
+        <v>259</v>
+      </c>
+      <c r="B509" s="7"/>
+      <c r="G509">
+        <v>507</v>
+      </c>
+      <c r="H509" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A510" s="7">
+        <v>259</v>
+      </c>
+      <c r="B510" s="7"/>
+      <c r="G510">
+        <v>508</v>
+      </c>
+      <c r="H510" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A511" s="7">
+        <v>259</v>
+      </c>
+      <c r="B511" s="7"/>
+      <c r="G511">
+        <v>509</v>
+      </c>
+      <c r="H511" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A512">
+        <v>256</v>
+      </c>
+      <c r="B512" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G512">
+        <v>510</v>
+      </c>
+      <c r="H512" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>256</v>
+      </c>
+      <c r="B513" s="6"/>
+      <c r="G513">
+        <v>511</v>
+      </c>
+      <c r="H513" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A514">
+        <v>262</v>
+      </c>
+      <c r="B514" s="6" t="s">
+        <v>1538</v>
+      </c>
+      <c r="G514">
+        <v>512</v>
+      </c>
+      <c r="H514" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A515">
+        <v>256</v>
+      </c>
+      <c r="B515" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G515">
+        <v>513</v>
+      </c>
+      <c r="H515" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A516">
+        <v>256</v>
+      </c>
+      <c r="B516" s="6"/>
+      <c r="G516">
+        <v>514</v>
+      </c>
+      <c r="H516" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A517">
+        <v>262</v>
+      </c>
+      <c r="B517" s="6" t="s">
+        <v>1538</v>
+      </c>
+      <c r="G517">
+        <v>515</v>
+      </c>
+      <c r="H517" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A518">
+        <v>264</v>
+      </c>
+      <c r="B518" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G518">
+        <v>516</v>
+      </c>
+      <c r="H518" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A519">
+        <v>264</v>
+      </c>
+      <c r="B519" s="6"/>
+      <c r="G519">
+        <v>517</v>
+      </c>
+      <c r="H519" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A520">
+        <v>259</v>
+      </c>
+      <c r="B520" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G520">
+        <v>518</v>
+      </c>
+      <c r="H520" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A521">
+        <v>259</v>
+      </c>
+      <c r="B521" s="6"/>
+      <c r="G521">
+        <v>519</v>
+      </c>
+      <c r="H521" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A522">
+        <v>259</v>
+      </c>
+      <c r="B522" s="6"/>
+      <c r="G522">
+        <v>520</v>
+      </c>
+      <c r="H522" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A523">
+        <v>256</v>
+      </c>
+      <c r="B523" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G523">
+        <v>521</v>
+      </c>
+      <c r="H523" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A524">
+        <v>256</v>
+      </c>
+      <c r="B524" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G524">
+        <v>522</v>
+      </c>
+      <c r="H524" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A525">
+        <v>256</v>
+      </c>
+      <c r="B525" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G525">
+        <v>523</v>
+      </c>
+      <c r="H525" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <v>256</v>
+      </c>
+      <c r="B526" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G526">
+        <v>524</v>
+      </c>
+      <c r="H526" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A527">
+        <v>256</v>
+      </c>
+      <c r="B527" s="6"/>
+      <c r="G527">
+        <v>525</v>
+      </c>
+      <c r="H527" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A528">
+        <v>256</v>
+      </c>
+      <c r="B528" s="6"/>
+      <c r="G528">
+        <v>526</v>
+      </c>
+      <c r="H528" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A529">
+        <v>256</v>
+      </c>
+      <c r="B529" s="6"/>
+      <c r="G529">
+        <v>527</v>
+      </c>
+      <c r="H529" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A530">
+        <v>256</v>
+      </c>
+      <c r="B530" s="6"/>
+      <c r="G530">
+        <v>528</v>
+      </c>
+      <c r="H530" t="s">
+        <v>1589</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>